<commit_message>
convert to plain text docx and doc
</commit_message>
<xml_diff>
--- a/task_refresh_xldb/рез2.xlsx
+++ b/task_refresh_xldb/рез2.xlsx
@@ -5207,10 +5207,10 @@
   <dimension ref="A1:AA49377"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <pane xSplit="14" ySplit="2" topLeftCell="O15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="14" ySplit="2" topLeftCell="V126" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="O1" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomRight" activeCell="N135" sqref="N135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
@@ -21635,7 +21635,7 @@
         <v>35400.044300000001</v>
       </c>
       <c r="W35" s="28" t="str">
-        <f t="shared" ref="W35:W66" ca="1" si="3">DATEDIF(V35,$N$1,"y")&amp;" р."</f>
+        <f t="shared" ref="W35:W57" ca="1" si="3">DATEDIF(V35,$N$1,"y")&amp;" р."</f>
         <v>28 р.</v>
       </c>
       <c r="X35" s="196">

</xml_diff>